<commit_message>
En el apartado de derechos existe una diferencia de $85,121,000, por lo cual no existirá una igual en el total entre la base original y la nueva base
</commit_message>
<xml_diff>
--- a/Presupuesto-Jalisco/2018-ingresos-autorizado/Ley de Ingresos del Estado de Jalisco para el ejercicio fiscal 2018.xlsx
+++ b/Presupuesto-Jalisco/2018-ingresos-autorizado/Ley de Ingresos del Estado de Jalisco para el ejercicio fiscal 2018.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\sepbr\app\webroot\files\Preciudadano\Autorizado2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GioVanny\Documents\Transversal-Presupuesto-Abierto\Presupuesto-Jalisco\2018-ingresos-autorizado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{373EDE31-B0E3-4617-9957-5D0690CE0FAD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C81F412-486B-45EE-8B05-41B59C16B037}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3825"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ingresos" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="210">
   <si>
     <t>Niveles de ingresos</t>
   </si>
@@ -511,12 +512,159 @@
   </si>
   <si>
     <t>4.03.04.01 Aportación Cruz Roja Mexicana y Hogar Cabañas</t>
+  </si>
+  <si>
+    <t>Sobre los Ingresos</t>
+  </si>
+  <si>
+    <t>Impuestos</t>
+  </si>
+  <si>
+    <t>Impuesto sobre Loterías, Rifas, Sorteos, Juegos con Apuesta y Concursos de Toda Clase</t>
+  </si>
+  <si>
+    <t>Impuesto sobre Enajenación y Distribución de Boletos de Rifas y Sorteos</t>
+  </si>
+  <si>
+    <t>Impuesto sobre Remuneraciones al Trabajo Personal no Subordinado</t>
+  </si>
+  <si>
+    <t>Sobre la producción, el consumo y las transacciones</t>
+  </si>
+  <si>
+    <t>Impuesto sobre Transmisiones Patrimoniales de Bienes Muebles</t>
+  </si>
+  <si>
+    <t>Impuesto sobre la Adquisición de Vehículos Automotores Usados</t>
+  </si>
+  <si>
+    <t>Impuesto sobre Negocios Jurídicos e Instrumentos Notariales (ejercicios anteriores)</t>
+  </si>
+  <si>
+    <t>Impuesto sobre Hospedaje</t>
+  </si>
+  <si>
+    <t>Sobre Nóminas y Asimilables</t>
+  </si>
+  <si>
+    <t>Impuesto sobre Nóminas</t>
+  </si>
+  <si>
+    <t>Accesorios</t>
+  </si>
+  <si>
+    <t>Accesorios generados por Adeudos de Impuestos</t>
+  </si>
+  <si>
+    <t>Sub tipo</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Ingreso</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Derechos</t>
+  </si>
+  <si>
+    <t>Derechos por la Prestación de Servicios</t>
+  </si>
+  <si>
+    <t>Registro Público de la Propiedad y de Comercio</t>
+  </si>
+  <si>
+    <t>Archivo de Instrumentos Públicos y Archivo General del Estado</t>
+  </si>
+  <si>
+    <t>Autorizaciones para el Ejercicio Profesional y Notarial</t>
+  </si>
+  <si>
+    <t>Servicios en los ramos de Movilidad y Transporte</t>
+  </si>
+  <si>
+    <t>Aportación Cruz Roja Mexicana y Hogar Cabañas</t>
+  </si>
+  <si>
+    <t>Certificaciones, Expediciones de Constancias y  Otros Servicios</t>
+  </si>
+  <si>
+    <t>Otros Derechos</t>
+  </si>
+  <si>
+    <t>Servicios diversos</t>
+  </si>
+  <si>
+    <t>Accesorios Generados por Adeudos de Derechos</t>
+  </si>
+  <si>
+    <t>Productos</t>
+  </si>
+  <si>
+    <t>Productos tipo Corriente</t>
+  </si>
+  <si>
+    <t>Uso, Goce, Aprovechamiento o Explotación de Bienes de Dominio Privado</t>
+  </si>
+  <si>
+    <t>Productos diversos</t>
+  </si>
+  <si>
+    <t>Productos de Capital</t>
+  </si>
+  <si>
+    <t>Rendimientos e Intereses de Capital e Inversiones del Estado</t>
+  </si>
+  <si>
+    <t>Aprovechamientos</t>
+  </si>
+  <si>
+    <t>Aprovechamientos de Tipo Corriente</t>
+  </si>
+  <si>
+    <t>Diversos</t>
+  </si>
+  <si>
+    <t>100% de la Recaudación de ISR que se entera a la Federación (ISR ESTATAL)</t>
+  </si>
+  <si>
+    <t>IEPS Gasolinas y Diesel</t>
+  </si>
+  <si>
+    <t>Incentivos derivados de la Colaboración Fiscal</t>
+  </si>
+  <si>
+    <t>Multas de Movilidad y Transporte</t>
+  </si>
+  <si>
+    <t>Participaciones y Aportaciones</t>
+  </si>
+  <si>
+    <t>Participaciones</t>
+  </si>
+  <si>
+    <t>Fondo General de Participaciones</t>
+  </si>
+  <si>
+    <t>Fondo de Fomento Municipal</t>
+  </si>
+  <si>
+    <t>Impuesto Especial sobre Producción y Servicios (Tabacos y Licores)</t>
+  </si>
+  <si>
+    <t>Fondo de Fiscalización y Recaudación</t>
+  </si>
+  <si>
+    <t>100% de la Recaudación de ISR que se entera a la Federación (ISR MUNICIPAL)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -528,12 +676,14 @@
       <sz val="15"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -561,7 +711,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -584,11 +734,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -612,19 +773,48 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -973,98 +1163,101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O109"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="I109" sqref="I109"/>
+    <sheetView topLeftCell="B47" workbookViewId="0">
+      <selection activeCell="H70" sqref="H70:H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="103.7109375" customWidth="1"/>
-    <col min="9" max="9" width="30" customWidth="1"/>
-    <col min="10" max="14" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="103.7109375" customWidth="1"/>
+    <col min="8" max="8" width="30" customWidth="1"/>
+    <col min="9" max="13" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-    </row>
-    <row r="2" spans="2:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+    </row>
+    <row r="2" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="1" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="I3" s="1">
+        <v>2019</v>
+      </c>
       <c r="J3" s="1">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="K3" s="1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="L3" s="1">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="M3" s="1">
-        <v>2022</v>
-      </c>
-      <c r="N3" s="1">
         <v>2023</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="12" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="4">
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="4">
         <v>4423216000</v>
       </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
       <c r="J4" s="3">
         <v>0</v>
       </c>
@@ -1077,22 +1270,22 @@
       <c r="M4" s="3">
         <v>0</v>
       </c>
-      <c r="N4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="D5" s="12" t="s">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="C5" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="4">
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="4">
         <v>340000000</v>
       </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
       <c r="J5" s="3">
         <v>0</v>
       </c>
@@ -1105,25 +1298,25 @@
       <c r="M5" s="3">
         <v>0</v>
       </c>
-      <c r="N5" s="3">
-        <v>0</v>
-      </c>
-      <c r="O5" s="5">
-        <f>SUM(I6:I8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="E6" s="12" t="s">
+      <c r="N5" s="5">
+        <f>SUM(H6:H8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="D6" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="3" t="s">
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
       <c r="J6" s="3">
         <v>0</v>
       </c>
@@ -1136,21 +1329,21 @@
       <c r="M6" s="3">
         <v>0</v>
       </c>
-      <c r="N6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="E7" s="12" t="s">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="D7" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="3" t="s">
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
       <c r="J7" s="3">
         <v>0</v>
       </c>
@@ -1163,21 +1356,21 @@
       <c r="M7" s="3">
         <v>0</v>
       </c>
-      <c r="N7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="E8" s="12" t="s">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="D8" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="3" t="s">
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
       <c r="J8" s="3">
         <v>0</v>
       </c>
@@ -1190,19 +1383,19 @@
       <c r="M8" s="3">
         <v>0</v>
       </c>
-      <c r="N8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="D9" s="12" t="s">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="C9" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
       <c r="I9" s="3">
         <v>0</v>
       </c>
@@ -1218,22 +1411,22 @@
       <c r="M9" s="3">
         <v>0</v>
       </c>
-      <c r="N9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="D10" s="12" t="s">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="C10" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="4">
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="4">
         <v>601359000</v>
       </c>
+      <c r="I10" s="3">
+        <v>0</v>
+      </c>
       <c r="J10" s="3">
         <v>0</v>
       </c>
@@ -1246,21 +1439,21 @@
       <c r="M10" s="3">
         <v>0</v>
       </c>
-      <c r="N10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="E11" s="12" t="s">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="D11" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="3" t="s">
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
       <c r="J11" s="3">
         <v>0</v>
       </c>
@@ -1273,21 +1466,21 @@
       <c r="M11" s="3">
         <v>0</v>
       </c>
-      <c r="N11" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="E12" s="12" t="s">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="D12" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="3" t="s">
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="I12" s="3">
+        <v>0</v>
+      </c>
       <c r="J12" s="3">
         <v>0</v>
       </c>
@@ -1300,21 +1493,21 @@
       <c r="M12" s="3">
         <v>0</v>
       </c>
-      <c r="N12" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="E13" s="12" t="s">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="D13" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="3" t="s">
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="I13" s="3">
+        <v>0</v>
+      </c>
       <c r="J13" s="3">
         <v>0</v>
       </c>
@@ -1327,21 +1520,21 @@
       <c r="M13" s="3">
         <v>0</v>
       </c>
-      <c r="N13" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="E14" s="12" t="s">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="D14" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="3" t="s">
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="I14" s="3">
+        <v>0</v>
+      </c>
       <c r="J14" s="3">
         <v>0</v>
       </c>
@@ -1354,19 +1547,19 @@
       <c r="M14" s="3">
         <v>0</v>
       </c>
-      <c r="N14" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="D15" s="12" t="s">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="C15" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
       <c r="I15" s="3">
         <v>0</v>
       </c>
@@ -1382,22 +1575,22 @@
       <c r="M15" s="3">
         <v>0</v>
       </c>
-      <c r="N15" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="D16" s="12" t="s">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="C16" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="3" t="s">
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
       <c r="J16" s="3">
         <v>0</v>
       </c>
@@ -1410,21 +1603,21 @@
       <c r="M16" s="3">
         <v>0</v>
       </c>
-      <c r="N16" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="E17" s="12" t="s">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="D17" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="3" t="s">
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="I17" s="3">
+        <v>0</v>
+      </c>
       <c r="J17" s="3">
         <v>0</v>
       </c>
@@ -1437,19 +1630,19 @@
       <c r="M17" s="3">
         <v>0</v>
       </c>
-      <c r="N17" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="D18" s="12" t="s">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="C18" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
       <c r="I18" s="3">
         <v>0</v>
       </c>
@@ -1465,22 +1658,22 @@
       <c r="M18" s="3">
         <v>0</v>
       </c>
-      <c r="N18" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="D19" s="12" t="s">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="C19" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="3" t="s">
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="I19" s="3">
+        <v>0</v>
+      </c>
       <c r="J19" s="3">
         <v>0</v>
       </c>
@@ -1493,21 +1686,21 @@
       <c r="M19" s="3">
         <v>0</v>
       </c>
-      <c r="N19" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-      <c r="E20" s="12" t="s">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="D20" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="3" t="s">
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="I20" s="3">
+        <v>0</v>
+      </c>
       <c r="J20" s="3">
         <v>0</v>
       </c>
@@ -1520,19 +1713,19 @@
       <c r="M20" s="3">
         <v>0</v>
       </c>
-      <c r="N20" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="D21" s="12" t="s">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="C21" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
       <c r="I21" s="3">
         <v>0</v>
       </c>
@@ -1548,19 +1741,19 @@
       <c r="M21" s="3">
         <v>0</v>
       </c>
-      <c r="N21" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="D22" s="12" t="s">
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="C22" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
       <c r="I22" s="3">
         <v>0</v>
       </c>
@@ -1576,20 +1769,20 @@
       <c r="M22" s="3">
         <v>0</v>
       </c>
-      <c r="N22" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="12" t="s">
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
       <c r="I23" s="3">
         <v>0</v>
       </c>
@@ -1605,20 +1798,20 @@
       <c r="M23" s="3">
         <v>0</v>
       </c>
-      <c r="N23" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="12" t="s">
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
       <c r="I24" s="3">
         <v>0</v>
       </c>
@@ -1634,23 +1827,23 @@
       <c r="M24" s="3">
         <v>0</v>
       </c>
-      <c r="N24" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="12" t="s">
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="4">
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="4">
         <v>3112408000</v>
       </c>
+      <c r="I25" s="3">
+        <v>0</v>
+      </c>
       <c r="J25" s="3">
         <v>0</v>
       </c>
@@ -1663,19 +1856,19 @@
       <c r="M25" s="3">
         <v>0</v>
       </c>
-      <c r="N25" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="D26" s="12" t="s">
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="C26" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="3">
+        <v>0</v>
+      </c>
       <c r="I26" s="3">
         <v>0</v>
       </c>
@@ -1691,19 +1884,19 @@
       <c r="M26" s="3">
         <v>0</v>
       </c>
-      <c r="N26" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="D27" s="12" t="s">
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="C27" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
       <c r="I27" s="3">
         <v>0</v>
       </c>
@@ -1719,22 +1912,22 @@
       <c r="M27" s="3">
         <v>0</v>
       </c>
-      <c r="N27" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="D28" s="12" t="s">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="C28" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="4">
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="4">
         <v>3014369000</v>
       </c>
+      <c r="I28" s="3">
+        <v>0</v>
+      </c>
       <c r="J28" s="3">
         <v>0</v>
       </c>
@@ -1747,21 +1940,21 @@
       <c r="M28" s="3">
         <v>0</v>
       </c>
-      <c r="N28" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
-      <c r="E29" s="12" t="s">
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="D29" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="3" t="s">
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="I29" s="3">
+        <v>0</v>
+      </c>
       <c r="J29" s="3">
         <v>0</v>
       </c>
@@ -1774,21 +1967,21 @@
       <c r="M29" s="3">
         <v>0</v>
       </c>
-      <c r="N29" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="E30" s="12" t="s">
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="D30" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="3" t="s">
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="I30" s="3">
+        <v>0</v>
+      </c>
       <c r="J30" s="3">
         <v>0</v>
       </c>
@@ -1801,21 +1994,21 @@
       <c r="M30" s="3">
         <v>0</v>
       </c>
-      <c r="N30" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-      <c r="E31" s="12" t="s">
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="D31" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="3" t="s">
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="I31" s="3">
+        <v>0</v>
+      </c>
       <c r="J31" s="3">
         <v>0</v>
       </c>
@@ -1828,21 +2021,21 @@
       <c r="M31" s="3">
         <v>0</v>
       </c>
-      <c r="N31" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="E32" s="12" t="s">
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="D32" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="3" t="s">
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="I32" s="3">
+        <v>0</v>
+      </c>
       <c r="J32" s="3">
         <v>0</v>
       </c>
@@ -1855,38 +2048,38 @@
       <c r="M32" s="3">
         <v>0</v>
       </c>
-      <c r="N32" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-      <c r="E33" s="12" t="s">
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="D33" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="7">
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="7">
         <v>85121000</v>
       </c>
+      <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B34" s="2"/>
-      <c r="E34" s="12" t="s">
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="D34" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="3" t="s">
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="I34" s="3">
+        <v>0</v>
+      </c>
       <c r="J34" s="3">
         <v>0</v>
       </c>
@@ -1899,22 +2092,22 @@
       <c r="M34" s="3">
         <v>0</v>
       </c>
-      <c r="N34" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="2"/>
-      <c r="D35" s="12" t="s">
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="C35" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="3" t="s">
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="I35" s="3">
+        <v>0</v>
+      </c>
       <c r="J35" s="3">
         <v>0</v>
       </c>
@@ -1927,21 +2120,21 @@
       <c r="M35" s="3">
         <v>0</v>
       </c>
-      <c r="N35" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B36" s="2"/>
-      <c r="E36" s="12" t="s">
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="D36" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="3" t="s">
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="I36" s="3">
+        <v>0</v>
+      </c>
       <c r="J36" s="3">
         <v>0</v>
       </c>
@@ -1954,22 +2147,22 @@
       <c r="M36" s="3">
         <v>0</v>
       </c>
-      <c r="N36" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="2"/>
-      <c r="D37" s="12" t="s">
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="C37" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="3" t="s">
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="I37" s="3">
+        <v>0</v>
+      </c>
       <c r="J37" s="3">
         <v>0</v>
       </c>
@@ -1982,21 +2175,21 @@
       <c r="M37" s="3">
         <v>0</v>
       </c>
-      <c r="N37" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B38" s="2"/>
-      <c r="E38" s="12" t="s">
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="D38" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="3" t="s">
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="I38" s="3">
+        <v>0</v>
+      </c>
       <c r="J38" s="3">
         <v>0</v>
       </c>
@@ -2009,19 +2202,19 @@
       <c r="M38" s="3">
         <v>0</v>
       </c>
-      <c r="N38" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B39" s="2"/>
-      <c r="D39" s="12" t="s">
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="C39" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="3">
+        <v>0</v>
+      </c>
       <c r="I39" s="3">
         <v>0</v>
       </c>
@@ -2037,23 +2230,23 @@
       <c r="M39" s="3">
         <v>0</v>
       </c>
-      <c r="N39" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B40" s="2"/>
-      <c r="C40" s="12" t="s">
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="4">
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="4">
         <v>171266000</v>
       </c>
+      <c r="I40" s="3">
+        <v>0</v>
+      </c>
       <c r="J40" s="3">
         <v>0</v>
       </c>
@@ -2066,22 +2259,22 @@
       <c r="M40" s="3">
         <v>0</v>
       </c>
-      <c r="N40" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B41" s="2"/>
-      <c r="D41" s="12" t="s">
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="C41" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="4">
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="4">
         <v>153895000</v>
       </c>
+      <c r="I41" s="3">
+        <v>0</v>
+      </c>
       <c r="J41" s="3">
         <v>0</v>
       </c>
@@ -2094,21 +2287,21 @@
       <c r="M41" s="3">
         <v>0</v>
       </c>
-      <c r="N41" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B42" s="2"/>
-      <c r="E42" s="12" t="s">
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="D42" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="3" t="s">
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="I42" s="3">
+        <v>0</v>
+      </c>
       <c r="J42" s="3">
         <v>0</v>
       </c>
@@ -2121,21 +2314,21 @@
       <c r="M42" s="3">
         <v>0</v>
       </c>
-      <c r="N42" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B43" s="2"/>
-      <c r="E43" s="12" t="s">
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="D43" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="3" t="s">
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="I43" s="3">
+        <v>0</v>
+      </c>
       <c r="J43" s="3">
         <v>0</v>
       </c>
@@ -2148,22 +2341,22 @@
       <c r="M43" s="3">
         <v>0</v>
       </c>
-      <c r="N43" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B44" s="2"/>
-      <c r="D44" s="12" t="s">
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="C44" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="10"/>
-      <c r="I44" s="3" t="s">
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="I44" s="3">
+        <v>0</v>
+      </c>
       <c r="J44" s="3">
         <v>0</v>
       </c>
@@ -2176,21 +2369,21 @@
       <c r="M44" s="3">
         <v>0</v>
       </c>
-      <c r="N44" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B45" s="2"/>
-      <c r="E45" s="12" t="s">
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="D45" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="10"/>
-      <c r="I45" s="3" t="s">
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="I45" s="3">
+        <v>0</v>
+      </c>
       <c r="J45" s="3">
         <v>0</v>
       </c>
@@ -2203,19 +2396,19 @@
       <c r="M45" s="3">
         <v>0</v>
       </c>
-      <c r="N45" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B46" s="2"/>
-      <c r="D46" s="12" t="s">
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="C46" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="10"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="3">
+        <v>0</v>
+      </c>
       <c r="I46" s="3">
         <v>0</v>
       </c>
@@ -2231,23 +2424,23 @@
       <c r="M46" s="3">
         <v>0</v>
       </c>
-      <c r="N46" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B47" s="2"/>
-      <c r="C47" s="12" t="s">
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
-      <c r="I47" s="4">
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="4">
         <v>10644169000</v>
       </c>
+      <c r="I47" s="3">
+        <v>0</v>
+      </c>
       <c r="J47" s="3">
         <v>0</v>
       </c>
@@ -2260,22 +2453,22 @@
       <c r="M47" s="3">
         <v>0</v>
       </c>
-      <c r="N47" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B48" s="2"/>
-      <c r="D48" s="12" t="s">
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="C48" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
-      <c r="I48" s="4">
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="4">
         <v>10644169000</v>
       </c>
+      <c r="I48" s="3">
+        <v>0</v>
+      </c>
       <c r="J48" s="3">
         <v>0</v>
       </c>
@@ -2288,21 +2481,21 @@
       <c r="M48" s="3">
         <v>0</v>
       </c>
-      <c r="N48" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B49" s="2"/>
-      <c r="E49" s="12" t="s">
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="D49" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
-      <c r="H49" s="10"/>
-      <c r="I49" s="3" t="s">
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="I49" s="3">
+        <v>0</v>
+      </c>
       <c r="J49" s="3">
         <v>0</v>
       </c>
@@ -2315,21 +2508,21 @@
       <c r="M49" s="3">
         <v>0</v>
       </c>
-      <c r="N49" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B50" s="2"/>
-      <c r="E50" s="12" t="s">
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="D50" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="3" t="s">
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="I50" s="3">
+        <v>0</v>
+      </c>
       <c r="J50" s="3">
         <v>0</v>
       </c>
@@ -2342,21 +2535,21 @@
       <c r="M50" s="3">
         <v>0</v>
       </c>
-      <c r="N50" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B51" s="2"/>
-      <c r="E51" s="12" t="s">
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="D51" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="F51" s="10"/>
-      <c r="G51" s="10"/>
-      <c r="H51" s="10"/>
-      <c r="I51" s="3" t="s">
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="I51" s="3">
+        <v>0</v>
+      </c>
       <c r="J51" s="3">
         <v>0</v>
       </c>
@@ -2369,21 +2562,21 @@
       <c r="M51" s="3">
         <v>0</v>
       </c>
-      <c r="N51" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B52" s="2"/>
-      <c r="E52" s="12" t="s">
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="D52" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="4">
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="4">
         <v>3077392000</v>
       </c>
+      <c r="I52" s="3">
+        <v>0</v>
+      </c>
       <c r="J52" s="3">
         <v>0</v>
       </c>
@@ -2396,20 +2589,20 @@
       <c r="M52" s="3">
         <v>0</v>
       </c>
-      <c r="N52" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B53" s="2"/>
-      <c r="F53" s="12" t="s">
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="E53" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="G53" s="10"/>
-      <c r="H53" s="10"/>
-      <c r="I53" s="3" t="s">
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="I53" s="3">
+        <v>0</v>
+      </c>
       <c r="J53" s="3">
         <v>0</v>
       </c>
@@ -2422,20 +2615,20 @@
       <c r="M53" s="3">
         <v>0</v>
       </c>
-      <c r="N53" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B54" s="2"/>
-      <c r="F54" s="12" t="s">
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+      <c r="E54" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="G54" s="10"/>
-      <c r="H54" s="10"/>
-      <c r="I54" s="3" t="s">
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="I54" s="3">
+        <v>0</v>
+      </c>
       <c r="J54" s="3">
         <v>0</v>
       </c>
@@ -2448,20 +2641,20 @@
       <c r="M54" s="3">
         <v>0</v>
       </c>
-      <c r="N54" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B55" s="2"/>
-      <c r="F55" s="12" t="s">
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+      <c r="E55" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="G55" s="10"/>
-      <c r="H55" s="10"/>
-      <c r="I55" s="3" t="s">
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="I55" s="3">
+        <v>0</v>
+      </c>
       <c r="J55" s="3">
         <v>0</v>
       </c>
@@ -2474,20 +2667,20 @@
       <c r="M55" s="3">
         <v>0</v>
       </c>
-      <c r="N55" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B56" s="2"/>
-      <c r="F56" s="12" t="s">
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+      <c r="E56" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="G56" s="10"/>
-      <c r="H56" s="10"/>
-      <c r="I56" s="3" t="s">
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="I56" s="3">
+        <v>0</v>
+      </c>
       <c r="J56" s="3">
         <v>0</v>
       </c>
@@ -2500,20 +2693,20 @@
       <c r="M56" s="3">
         <v>0</v>
       </c>
-      <c r="N56" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B57" s="2"/>
-      <c r="F57" s="12" t="s">
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+      <c r="E57" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="G57" s="10"/>
-      <c r="H57" s="10"/>
-      <c r="I57" s="4">
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="4">
         <v>1738688000</v>
       </c>
+      <c r="I57" s="3">
+        <v>0</v>
+      </c>
       <c r="J57" s="3">
         <v>0</v>
       </c>
@@ -2526,19 +2719,19 @@
       <c r="M57" s="3">
         <v>0</v>
       </c>
-      <c r="N57" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B58" s="2"/>
-      <c r="G58" s="12" t="s">
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+      <c r="F58" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="H58" s="10"/>
-      <c r="I58" s="3" t="s">
+      <c r="G58" s="12"/>
+      <c r="H58" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="I58" s="3">
+        <v>0</v>
+      </c>
       <c r="J58" s="3">
         <v>0</v>
       </c>
@@ -2551,19 +2744,19 @@
       <c r="M58" s="3">
         <v>0</v>
       </c>
-      <c r="N58" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B59" s="2"/>
-      <c r="G59" s="12" t="s">
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+      <c r="F59" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="H59" s="10"/>
-      <c r="I59" s="3" t="s">
+      <c r="G59" s="12"/>
+      <c r="H59" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="I59" s="3">
+        <v>0</v>
+      </c>
       <c r="J59" s="3">
         <v>0</v>
       </c>
@@ -2576,19 +2769,19 @@
       <c r="M59" s="3">
         <v>0</v>
       </c>
-      <c r="N59" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B60" s="2"/>
-      <c r="G60" s="12" t="s">
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="F60" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="H60" s="10"/>
-      <c r="I60" s="3" t="s">
+      <c r="G60" s="12"/>
+      <c r="H60" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="I60" s="3">
+        <v>0</v>
+      </c>
       <c r="J60" s="3">
         <v>0</v>
       </c>
@@ -2601,21 +2794,21 @@
       <c r="M60" s="3">
         <v>0</v>
       </c>
-      <c r="N60" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B61" s="2"/>
-      <c r="E61" s="12" t="s">
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+      <c r="D61" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="F61" s="10"/>
-      <c r="G61" s="10"/>
-      <c r="H61" s="10"/>
-      <c r="I61" s="6" t="s">
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="6" t="s">
         <v>31</v>
       </c>
+      <c r="I61" s="3">
+        <v>0</v>
+      </c>
       <c r="J61" s="3">
         <v>0</v>
       </c>
@@ -2628,19 +2821,19 @@
       <c r="M61" s="3">
         <v>0</v>
       </c>
-      <c r="N61" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B62" s="2"/>
-      <c r="D62" s="12" t="s">
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="C62" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
-      <c r="G62" s="10"/>
-      <c r="H62" s="10"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="3">
+        <v>0</v>
+      </c>
       <c r="I62" s="3">
         <v>0</v>
       </c>
@@ -2656,19 +2849,19 @@
       <c r="M62" s="3">
         <v>0</v>
       </c>
-      <c r="N62" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B63" s="2"/>
-      <c r="D63" s="12" t="s">
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+      <c r="C63" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="E63" s="10"/>
-      <c r="F63" s="10"/>
-      <c r="G63" s="10"/>
-      <c r="H63" s="10"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="3">
+        <v>0</v>
+      </c>
       <c r="I63" s="3">
         <v>0</v>
       </c>
@@ -2684,96 +2877,96 @@
       <c r="M63" s="3">
         <v>0</v>
       </c>
-      <c r="N63" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B64" s="2"/>
-      <c r="C64" s="12" t="s">
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+      <c r="B64" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="10"/>
-      <c r="H64" s="10"/>
-      <c r="I64" s="3">
-        <v>0</v>
-      </c>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="3">
+        <v>0</v>
+      </c>
+      <c r="I64" s="3"/>
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
       <c r="M64" s="3"/>
-      <c r="N64" s="3"/>
-    </row>
-    <row r="65" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B65" s="2"/>
-      <c r="D65" s="13" t="s">
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+      <c r="C65" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="3">
-        <v>0</v>
-      </c>
+      <c r="D65" s="16"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="3">
+        <v>0</v>
+      </c>
+      <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
       <c r="M65" s="3"/>
-      <c r="N65" s="3"/>
-    </row>
-    <row r="66" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B66" s="2"/>
-      <c r="D66" s="13" t="s">
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+      <c r="C66" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="3">
-        <v>0</v>
-      </c>
+      <c r="D66" s="16"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="3">
+        <v>0</v>
+      </c>
+      <c r="I66" s="3"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
       <c r="M66" s="3"/>
-      <c r="N66" s="3"/>
-    </row>
-    <row r="67" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B67" s="2"/>
-      <c r="D67" s="13" t="s">
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
+      <c r="C67" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="3">
-        <v>0</v>
-      </c>
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="3">
+        <v>0</v>
+      </c>
+      <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
       <c r="M67" s="3"/>
-      <c r="N67" s="3"/>
-    </row>
-    <row r="68" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B68" s="2"/>
-      <c r="C68" s="12" t="s">
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+      <c r="B68" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D68" s="10"/>
-      <c r="E68" s="10"/>
-      <c r="F68" s="10"/>
-      <c r="G68" s="10"/>
-      <c r="H68" s="10"/>
-      <c r="I68" s="4">
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
+      <c r="H68" s="4">
         <v>79019990000</v>
       </c>
+      <c r="I68" s="3">
+        <v>0</v>
+      </c>
       <c r="J68" s="3">
         <v>0</v>
       </c>
@@ -2786,22 +2979,22 @@
       <c r="M68" s="3">
         <v>0</v>
       </c>
-      <c r="N68" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B69" s="2"/>
-      <c r="D69" s="12" t="s">
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" s="2"/>
+      <c r="C69" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="E69" s="10"/>
-      <c r="F69" s="10"/>
-      <c r="G69" s="10"/>
-      <c r="H69" s="10"/>
-      <c r="I69" s="4">
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
+      <c r="H69" s="4">
         <v>45088177000</v>
       </c>
+      <c r="I69" s="3">
+        <v>0</v>
+      </c>
       <c r="J69" s="3">
         <v>0</v>
       </c>
@@ -2814,21 +3007,21 @@
       <c r="M69" s="3">
         <v>0</v>
       </c>
-      <c r="N69" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B70" s="2"/>
-      <c r="E70" s="12" t="s">
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
+      <c r="D70" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="F70" s="10"/>
-      <c r="G70" s="10"/>
-      <c r="H70" s="10"/>
-      <c r="I70" s="3" t="s">
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="12"/>
+      <c r="H70" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="I70" s="3">
+        <v>0</v>
+      </c>
       <c r="J70" s="3">
         <v>0</v>
       </c>
@@ -2841,21 +3034,21 @@
       <c r="M70" s="3">
         <v>0</v>
       </c>
-      <c r="N70" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B71" s="2"/>
-      <c r="E71" s="12" t="s">
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" s="2"/>
+      <c r="D71" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="F71" s="10"/>
-      <c r="G71" s="10"/>
-      <c r="H71" s="10"/>
-      <c r="I71" s="3" t="s">
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="I71" s="3">
+        <v>0</v>
+      </c>
       <c r="J71" s="3">
         <v>0</v>
       </c>
@@ -2868,21 +3061,21 @@
       <c r="M71" s="3">
         <v>0</v>
       </c>
-      <c r="N71" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B72" s="2"/>
-      <c r="E72" s="12" t="s">
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" s="2"/>
+      <c r="D72" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="F72" s="10"/>
-      <c r="G72" s="10"/>
-      <c r="H72" s="10"/>
-      <c r="I72" s="3" t="s">
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="I72" s="3">
+        <v>0</v>
+      </c>
       <c r="J72" s="3">
         <v>0</v>
       </c>
@@ -2895,21 +3088,21 @@
       <c r="M72" s="3">
         <v>0</v>
       </c>
-      <c r="N72" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B73" s="2"/>
-      <c r="E73" s="12" t="s">
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="2"/>
+      <c r="D73" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="F73" s="10"/>
-      <c r="G73" s="10"/>
-      <c r="H73" s="10"/>
-      <c r="I73" s="3" t="s">
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="12"/>
+      <c r="H73" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="I73" s="3">
+        <v>0</v>
+      </c>
       <c r="J73" s="3">
         <v>0</v>
       </c>
@@ -2922,21 +3115,21 @@
       <c r="M73" s="3">
         <v>0</v>
       </c>
-      <c r="N73" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B74" s="2"/>
-      <c r="E74" s="12" t="s">
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" s="2"/>
+      <c r="D74" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="F74" s="10"/>
-      <c r="G74" s="10"/>
-      <c r="H74" s="10"/>
-      <c r="I74" s="3" t="s">
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
+      <c r="H74" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="I74" s="3">
+        <v>0</v>
+      </c>
       <c r="J74" s="3">
         <v>0</v>
       </c>
@@ -2949,22 +3142,22 @@
       <c r="M74" s="3">
         <v>0</v>
       </c>
-      <c r="N74" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B75" s="2"/>
-      <c r="D75" s="12" t="s">
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" s="2"/>
+      <c r="C75" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="E75" s="10"/>
-      <c r="F75" s="10"/>
-      <c r="G75" s="10"/>
-      <c r="H75" s="10"/>
-      <c r="I75" s="4">
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
+      <c r="H75" s="4">
         <v>33931813000</v>
       </c>
+      <c r="I75" s="3">
+        <v>0</v>
+      </c>
       <c r="J75" s="3">
         <v>0</v>
       </c>
@@ -2977,21 +3170,21 @@
       <c r="M75" s="3">
         <v>0</v>
       </c>
-      <c r="N75" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B76" s="2"/>
-      <c r="E76" s="12" t="s">
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" s="2"/>
+      <c r="D76" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="F76" s="10"/>
-      <c r="G76" s="10"/>
-      <c r="H76" s="10"/>
-      <c r="I76" s="3" t="s">
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="I76" s="3">
+        <v>0</v>
+      </c>
       <c r="J76" s="3">
         <v>0</v>
       </c>
@@ -3004,21 +3197,21 @@
       <c r="M76" s="3">
         <v>0</v>
       </c>
-      <c r="N76" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B77" s="2"/>
-      <c r="E77" s="12" t="s">
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77" s="2"/>
+      <c r="D77" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="F77" s="10"/>
-      <c r="G77" s="10"/>
-      <c r="H77" s="10"/>
-      <c r="I77" s="3" t="s">
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="12"/>
+      <c r="H77" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="I77" s="3">
+        <v>0</v>
+      </c>
       <c r="J77" s="3">
         <v>0</v>
       </c>
@@ -3031,21 +3224,21 @@
       <c r="M77" s="3">
         <v>0</v>
       </c>
-      <c r="N77" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B78" s="2"/>
-      <c r="E78" s="12" t="s">
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78" s="2"/>
+      <c r="D78" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="F78" s="10"/>
-      <c r="G78" s="10"/>
-      <c r="H78" s="10"/>
-      <c r="I78" s="4">
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="12"/>
+      <c r="H78" s="4">
         <v>1773578000</v>
       </c>
+      <c r="I78" s="3">
+        <v>0</v>
+      </c>
       <c r="J78" s="3">
         <v>0</v>
       </c>
@@ -3058,20 +3251,20 @@
       <c r="M78" s="3">
         <v>0</v>
       </c>
-      <c r="N78" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B79" s="2"/>
-      <c r="F79" s="12" t="s">
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79" s="2"/>
+      <c r="E79" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="G79" s="10"/>
-      <c r="H79" s="10"/>
-      <c r="I79" s="3" t="s">
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
+      <c r="H79" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="I79" s="3">
+        <v>0</v>
+      </c>
       <c r="J79" s="3">
         <v>0</v>
       </c>
@@ -3084,20 +3277,20 @@
       <c r="M79" s="3">
         <v>0</v>
       </c>
-      <c r="N79" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B80" s="2"/>
-      <c r="F80" s="12" t="s">
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80" s="2"/>
+      <c r="E80" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="G80" s="10"/>
-      <c r="H80" s="10"/>
-      <c r="I80" s="3" t="s">
+      <c r="F80" s="12"/>
+      <c r="G80" s="12"/>
+      <c r="H80" s="3" t="s">
         <v>40</v>
       </c>
+      <c r="I80" s="3">
+        <v>0</v>
+      </c>
       <c r="J80" s="3">
         <v>0</v>
       </c>
@@ -3110,21 +3303,21 @@
       <c r="M80" s="3">
         <v>0</v>
       </c>
-      <c r="N80" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B81" s="2"/>
-      <c r="E81" s="12" t="s">
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81" s="2"/>
+      <c r="D81" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="F81" s="10"/>
-      <c r="G81" s="10"/>
-      <c r="H81" s="10"/>
-      <c r="I81" s="3" t="s">
+      <c r="E81" s="12"/>
+      <c r="F81" s="12"/>
+      <c r="G81" s="12"/>
+      <c r="H81" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="I81" s="3">
+        <v>0</v>
+      </c>
       <c r="J81" s="3">
         <v>0</v>
       </c>
@@ -3137,21 +3330,21 @@
       <c r="M81" s="3">
         <v>0</v>
       </c>
-      <c r="N81" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B82" s="2"/>
-      <c r="E82" s="12" t="s">
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82" s="2"/>
+      <c r="D82" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F82" s="10"/>
-      <c r="G82" s="10"/>
-      <c r="H82" s="10"/>
-      <c r="I82" s="4">
+      <c r="E82" s="12"/>
+      <c r="F82" s="12"/>
+      <c r="G82" s="12"/>
+      <c r="H82" s="4">
         <v>1105592000</v>
       </c>
+      <c r="I82" s="3">
+        <v>0</v>
+      </c>
       <c r="J82" s="3">
         <v>0</v>
       </c>
@@ -3164,20 +3357,20 @@
       <c r="M82" s="3">
         <v>0</v>
       </c>
-      <c r="N82" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B83" s="2"/>
-      <c r="F83" s="12" t="s">
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83" s="2"/>
+      <c r="E83" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="G83" s="10"/>
-      <c r="H83" s="10"/>
-      <c r="I83" s="3" t="s">
+      <c r="F83" s="12"/>
+      <c r="G83" s="12"/>
+      <c r="H83" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="I83" s="3">
+        <v>0</v>
+      </c>
       <c r="J83" s="3">
         <v>0</v>
       </c>
@@ -3190,36 +3383,36 @@
       <c r="M83" s="3">
         <v>0</v>
       </c>
-      <c r="N83" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B84" s="2"/>
-      <c r="F84" s="12" t="s">
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A84" s="2"/>
+      <c r="E84" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="G84" s="10"/>
-      <c r="H84" s="10"/>
-      <c r="I84" s="3" t="s">
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
+      <c r="H84" s="3" t="s">
         <v>44</v>
       </c>
+      <c r="I84" s="3"/>
       <c r="J84" s="3"/>
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
       <c r="M84" s="3"/>
-      <c r="N84" s="3"/>
-    </row>
-    <row r="85" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B85" s="2"/>
-      <c r="F85" s="12" t="s">
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A85" s="2"/>
+      <c r="E85" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="G85" s="10"/>
-      <c r="H85" s="10"/>
-      <c r="I85" s="3" t="s">
+      <c r="F85" s="12"/>
+      <c r="G85" s="12"/>
+      <c r="H85" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="I85" s="3">
+        <v>0</v>
+      </c>
       <c r="J85" s="3">
         <v>0</v>
       </c>
@@ -3232,20 +3425,20 @@
       <c r="M85" s="3">
         <v>0</v>
       </c>
-      <c r="N85" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B86" s="2"/>
-      <c r="F86" s="12" t="s">
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A86" s="2"/>
+      <c r="E86" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="G86" s="10"/>
-      <c r="H86" s="10"/>
-      <c r="I86" s="3" t="s">
+      <c r="F86" s="12"/>
+      <c r="G86" s="12"/>
+      <c r="H86" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="I86" s="3">
+        <v>0</v>
+      </c>
       <c r="J86" s="3">
         <v>0</v>
       </c>
@@ -3258,21 +3451,21 @@
       <c r="M86" s="3">
         <v>0</v>
       </c>
-      <c r="N86" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B87" s="2"/>
-      <c r="E87" s="12" t="s">
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A87" s="2"/>
+      <c r="D87" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="F87" s="10"/>
-      <c r="G87" s="10"/>
-      <c r="H87" s="10"/>
-      <c r="I87" s="3" t="s">
+      <c r="E87" s="12"/>
+      <c r="F87" s="12"/>
+      <c r="G87" s="12"/>
+      <c r="H87" s="3" t="s">
         <v>46</v>
       </c>
+      <c r="I87" s="3">
+        <v>0</v>
+      </c>
       <c r="J87" s="3">
         <v>0</v>
       </c>
@@ -3285,21 +3478,21 @@
       <c r="M87" s="3">
         <v>0</v>
       </c>
-      <c r="N87" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B88" s="2"/>
-      <c r="E88" s="12" t="s">
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88" s="2"/>
+      <c r="D88" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="F88" s="10"/>
-      <c r="G88" s="10"/>
-      <c r="H88" s="10"/>
-      <c r="I88" s="4">
+      <c r="E88" s="12"/>
+      <c r="F88" s="12"/>
+      <c r="G88" s="12"/>
+      <c r="H88" s="4">
         <v>362977000</v>
       </c>
+      <c r="I88" s="3">
+        <v>0</v>
+      </c>
       <c r="J88" s="3">
         <v>0</v>
       </c>
@@ -3312,20 +3505,20 @@
       <c r="M88" s="3">
         <v>0</v>
       </c>
-      <c r="N88" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B89" s="2"/>
-      <c r="F89" s="12" t="s">
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89" s="2"/>
+      <c r="E89" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="G89" s="10"/>
-      <c r="H89" s="10"/>
-      <c r="I89" s="3" t="s">
+      <c r="F89" s="12"/>
+      <c r="G89" s="12"/>
+      <c r="H89" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="I89" s="3">
+        <v>0</v>
+      </c>
       <c r="J89" s="3">
         <v>0</v>
       </c>
@@ -3338,20 +3531,20 @@
       <c r="M89" s="3">
         <v>0</v>
       </c>
-      <c r="N89" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B90" s="2"/>
-      <c r="F90" s="12" t="s">
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A90" s="2"/>
+      <c r="E90" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="G90" s="10"/>
-      <c r="H90" s="10"/>
-      <c r="I90" s="3" t="s">
+      <c r="F90" s="12"/>
+      <c r="G90" s="12"/>
+      <c r="H90" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="I90" s="3">
+        <v>0</v>
+      </c>
       <c r="J90" s="3">
         <v>0</v>
       </c>
@@ -3364,21 +3557,21 @@
       <c r="M90" s="3">
         <v>0</v>
       </c>
-      <c r="N90" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B91" s="2"/>
-      <c r="E91" s="12" t="s">
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A91" s="2"/>
+      <c r="D91" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="F91" s="10"/>
-      <c r="G91" s="10"/>
-      <c r="H91" s="10"/>
-      <c r="I91" s="3" t="s">
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="12"/>
+      <c r="H91" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="I91" s="3">
+        <v>0</v>
+      </c>
       <c r="J91" s="3">
         <v>0</v>
       </c>
@@ -3391,19 +3584,19 @@
       <c r="M91" s="3">
         <v>0</v>
       </c>
-      <c r="N91" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B92" s="2"/>
-      <c r="D92" s="12" t="s">
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A92" s="2"/>
+      <c r="C92" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="E92" s="10"/>
-      <c r="F92" s="10"/>
-      <c r="G92" s="10"/>
-      <c r="H92" s="10"/>
+      <c r="D92" s="12"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="12"/>
+      <c r="G92" s="12"/>
+      <c r="H92" s="3">
+        <v>0</v>
+      </c>
       <c r="I92" s="3">
         <v>0</v>
       </c>
@@ -3419,23 +3612,23 @@
       <c r="M92" s="3">
         <v>0</v>
       </c>
-      <c r="N92" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B93" s="2"/>
-      <c r="C93" s="12" t="s">
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A93" s="2"/>
+      <c r="B93" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="D93" s="10"/>
-      <c r="E93" s="10"/>
-      <c r="F93" s="10"/>
-      <c r="G93" s="10"/>
-      <c r="H93" s="10"/>
-      <c r="I93" s="4">
+      <c r="C93" s="12"/>
+      <c r="D93" s="12"/>
+      <c r="E93" s="12"/>
+      <c r="F93" s="12"/>
+      <c r="G93" s="12"/>
+      <c r="H93" s="4">
         <v>10937958000</v>
       </c>
+      <c r="I93" s="3">
+        <v>0</v>
+      </c>
       <c r="J93" s="3">
         <v>0</v>
       </c>
@@ -3448,22 +3641,22 @@
       <c r="M93" s="3">
         <v>0</v>
       </c>
-      <c r="N93" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B94" s="2"/>
-      <c r="D94" s="12" t="s">
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A94" s="2"/>
+      <c r="C94" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="E94" s="10"/>
-      <c r="F94" s="10"/>
-      <c r="G94" s="10"/>
-      <c r="H94" s="10"/>
-      <c r="I94" s="4">
+      <c r="D94" s="12"/>
+      <c r="E94" s="12"/>
+      <c r="F94" s="12"/>
+      <c r="G94" s="12"/>
+      <c r="H94" s="4">
         <v>10937958000</v>
       </c>
+      <c r="I94" s="3">
+        <v>0</v>
+      </c>
       <c r="J94" s="3">
         <v>0</v>
       </c>
@@ -3476,21 +3669,21 @@
       <c r="M94" s="3">
         <v>0</v>
       </c>
-      <c r="N94" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B95" s="2"/>
-      <c r="E95" s="12" t="s">
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A95" s="2"/>
+      <c r="D95" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="F95" s="10"/>
-      <c r="G95" s="10"/>
-      <c r="H95" s="10"/>
-      <c r="I95" s="3" t="s">
+      <c r="E95" s="12"/>
+      <c r="F95" s="12"/>
+      <c r="G95" s="12"/>
+      <c r="H95" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="I95" s="3">
+        <v>0</v>
+      </c>
       <c r="J95" s="3">
         <v>0</v>
       </c>
@@ -3503,21 +3696,21 @@
       <c r="M95" s="3">
         <v>0</v>
       </c>
-      <c r="N95" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B96" s="2"/>
-      <c r="E96" s="12" t="s">
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A96" s="2"/>
+      <c r="D96" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="F96" s="10"/>
-      <c r="G96" s="10"/>
-      <c r="H96" s="10"/>
-      <c r="I96" s="3" t="s">
+      <c r="E96" s="12"/>
+      <c r="F96" s="12"/>
+      <c r="G96" s="12"/>
+      <c r="H96" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="I96" s="3">
+        <v>0</v>
+      </c>
       <c r="J96" s="3">
         <v>0</v>
       </c>
@@ -3530,21 +3723,21 @@
       <c r="M96" s="3">
         <v>0</v>
       </c>
-      <c r="N96" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B97" s="2"/>
-      <c r="E97" s="12" t="s">
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A97" s="2"/>
+      <c r="D97" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="F97" s="10"/>
-      <c r="G97" s="10"/>
-      <c r="H97" s="10"/>
-      <c r="I97" s="3" t="s">
+      <c r="E97" s="12"/>
+      <c r="F97" s="12"/>
+      <c r="G97" s="12"/>
+      <c r="H97" s="3" t="s">
         <v>52</v>
       </c>
+      <c r="I97" s="3">
+        <v>0</v>
+      </c>
       <c r="J97" s="3">
         <v>0</v>
       </c>
@@ -3557,19 +3750,19 @@
       <c r="M97" s="3">
         <v>0</v>
       </c>
-      <c r="N97" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B98" s="2"/>
-      <c r="D98" s="12" t="s">
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A98" s="2"/>
+      <c r="C98" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="E98" s="10"/>
-      <c r="F98" s="10"/>
-      <c r="G98" s="10"/>
-      <c r="H98" s="10"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
+      <c r="G98" s="12"/>
+      <c r="H98" s="3">
+        <v>0</v>
+      </c>
       <c r="I98" s="3">
         <v>0</v>
       </c>
@@ -3585,19 +3778,19 @@
       <c r="M98" s="3">
         <v>0</v>
       </c>
-      <c r="N98" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B99" s="2"/>
-      <c r="D99" s="12" t="s">
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A99" s="2"/>
+      <c r="C99" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="E99" s="10"/>
-      <c r="F99" s="10"/>
-      <c r="G99" s="10"/>
-      <c r="H99" s="10"/>
+      <c r="D99" s="12"/>
+      <c r="E99" s="12"/>
+      <c r="F99" s="12"/>
+      <c r="G99" s="12"/>
+      <c r="H99" s="3">
+        <v>0</v>
+      </c>
       <c r="I99" s="3">
         <v>0</v>
       </c>
@@ -3613,19 +3806,19 @@
       <c r="M99" s="3">
         <v>0</v>
       </c>
-      <c r="N99" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B100" s="2"/>
-      <c r="D100" s="12" t="s">
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A100" s="2"/>
+      <c r="C100" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="E100" s="10"/>
-      <c r="F100" s="10"/>
-      <c r="G100" s="10"/>
-      <c r="H100" s="10"/>
+      <c r="D100" s="12"/>
+      <c r="E100" s="12"/>
+      <c r="F100" s="12"/>
+      <c r="G100" s="12"/>
+      <c r="H100" s="3">
+        <v>0</v>
+      </c>
       <c r="I100" s="3">
         <v>0</v>
       </c>
@@ -3641,19 +3834,19 @@
       <c r="M100" s="3">
         <v>0</v>
       </c>
-      <c r="N100" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B101" s="2"/>
-      <c r="D101" s="12" t="s">
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A101" s="2"/>
+      <c r="C101" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E101" s="10"/>
-      <c r="F101" s="10"/>
-      <c r="G101" s="10"/>
-      <c r="H101" s="10"/>
+      <c r="D101" s="12"/>
+      <c r="E101" s="12"/>
+      <c r="F101" s="12"/>
+      <c r="G101" s="12"/>
+      <c r="H101" s="3">
+        <v>0</v>
+      </c>
       <c r="I101" s="3">
         <v>0</v>
       </c>
@@ -3669,19 +3862,19 @@
       <c r="M101" s="3">
         <v>0</v>
       </c>
-      <c r="N101" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B102" s="2"/>
-      <c r="D102" s="12" t="s">
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A102" s="2"/>
+      <c r="C102" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="E102" s="10"/>
-      <c r="F102" s="10"/>
-      <c r="G102" s="10"/>
-      <c r="H102" s="10"/>
+      <c r="D102" s="12"/>
+      <c r="E102" s="12"/>
+      <c r="F102" s="12"/>
+      <c r="G102" s="12"/>
+      <c r="H102" s="3">
+        <v>0</v>
+      </c>
       <c r="I102" s="3">
         <v>0</v>
       </c>
@@ -3697,20 +3890,20 @@
       <c r="M102" s="3">
         <v>0</v>
       </c>
-      <c r="N102" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B103" s="2"/>
-      <c r="C103" s="12" t="s">
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A103" s="2"/>
+      <c r="B103" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="D103" s="10"/>
-      <c r="E103" s="10"/>
-      <c r="F103" s="10"/>
-      <c r="G103" s="10"/>
-      <c r="H103" s="10"/>
+      <c r="C103" s="12"/>
+      <c r="D103" s="12"/>
+      <c r="E103" s="12"/>
+      <c r="F103" s="12"/>
+      <c r="G103" s="12"/>
+      <c r="H103" s="3">
+        <v>0</v>
+      </c>
       <c r="I103" s="3">
         <v>0</v>
       </c>
@@ -3726,19 +3919,19 @@
       <c r="M103" s="3">
         <v>0</v>
       </c>
-      <c r="N103" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B104" s="2"/>
-      <c r="D104" s="12" t="s">
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A104" s="2"/>
+      <c r="C104" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="E104" s="10"/>
-      <c r="F104" s="10"/>
-      <c r="G104" s="10"/>
-      <c r="H104" s="10"/>
+      <c r="D104" s="12"/>
+      <c r="E104" s="12"/>
+      <c r="F104" s="12"/>
+      <c r="G104" s="12"/>
+      <c r="H104" s="3">
+        <v>0</v>
+      </c>
       <c r="I104" s="3">
         <v>0</v>
       </c>
@@ -3754,18 +3947,18 @@
       <c r="M104" s="3">
         <v>0</v>
       </c>
-      <c r="N104" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B105" s="2"/>
-      <c r="E105" s="12" t="s">
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A105" s="2"/>
+      <c r="D105" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="F105" s="10"/>
-      <c r="G105" s="10"/>
-      <c r="H105" s="10"/>
+      <c r="E105" s="12"/>
+      <c r="F105" s="12"/>
+      <c r="G105" s="12"/>
+      <c r="H105" s="3">
+        <v>0</v>
+      </c>
       <c r="I105" s="3">
         <v>0</v>
       </c>
@@ -3781,18 +3974,18 @@
       <c r="M105" s="3">
         <v>0</v>
       </c>
-      <c r="N105" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B106" s="2"/>
-      <c r="E106" s="12" t="s">
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
+      <c r="D106" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="F106" s="10"/>
-      <c r="G106" s="10"/>
-      <c r="H106" s="10"/>
+      <c r="E106" s="12"/>
+      <c r="F106" s="12"/>
+      <c r="G106" s="12"/>
+      <c r="H106" s="3">
+        <v>0</v>
+      </c>
       <c r="I106" s="3">
         <v>0</v>
       </c>
@@ -3808,18 +4001,18 @@
       <c r="M106" s="3">
         <v>0</v>
       </c>
-      <c r="N106" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B107" s="2"/>
-      <c r="E107" s="12" t="s">
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A107" s="2"/>
+      <c r="D107" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="F107" s="10"/>
-      <c r="G107" s="10"/>
-      <c r="H107" s="10"/>
+      <c r="E107" s="12"/>
+      <c r="F107" s="12"/>
+      <c r="G107" s="12"/>
+      <c r="H107" s="3">
+        <v>0</v>
+      </c>
       <c r="I107" s="3">
         <v>0</v>
       </c>
@@ -3835,19 +4028,19 @@
       <c r="M107" s="3">
         <v>0</v>
       </c>
-      <c r="N107" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B108" s="2"/>
-      <c r="D108" s="12" t="s">
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A108" s="2"/>
+      <c r="C108" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="E108" s="10"/>
-      <c r="F108" s="10"/>
-      <c r="G108" s="10"/>
-      <c r="H108" s="10"/>
+      <c r="D108" s="12"/>
+      <c r="E108" s="12"/>
+      <c r="F108" s="12"/>
+      <c r="G108" s="12"/>
+      <c r="H108" s="3">
+        <v>0</v>
+      </c>
       <c r="I108" s="3">
         <v>0</v>
       </c>
@@ -3863,23 +4056,23 @@
       <c r="M108" s="3">
         <v>0</v>
       </c>
-      <c r="N108" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B109" s="13" t="s">
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A109" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="C109" s="14"/>
-      <c r="D109" s="14"/>
-      <c r="E109" s="14"/>
-      <c r="F109" s="14"/>
-      <c r="G109" s="14"/>
-      <c r="H109" s="14"/>
-      <c r="I109" s="8">
+      <c r="B109" s="16"/>
+      <c r="C109" s="16"/>
+      <c r="D109" s="16"/>
+      <c r="E109" s="16"/>
+      <c r="F109" s="16"/>
+      <c r="G109" s="16"/>
+      <c r="H109" s="8">
         <v>108309007000</v>
       </c>
+      <c r="I109" s="3">
+        <v>0</v>
+      </c>
       <c r="J109" s="3">
         <v>0</v>
       </c>
@@ -3890,127 +4083,584 @@
         <v>0</v>
       </c>
       <c r="M109" s="3">
-        <v>0</v>
-      </c>
-      <c r="N109" s="3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="109">
-    <mergeCell ref="B109:H109"/>
-    <mergeCell ref="E107:H107"/>
-    <mergeCell ref="D108:H108"/>
-    <mergeCell ref="E33:H33"/>
-    <mergeCell ref="C64:H64"/>
-    <mergeCell ref="D65:H65"/>
-    <mergeCell ref="D66:H66"/>
-    <mergeCell ref="D67:H67"/>
-    <mergeCell ref="D101:H101"/>
-    <mergeCell ref="D102:H102"/>
-    <mergeCell ref="D104:H104"/>
-    <mergeCell ref="E105:H105"/>
-    <mergeCell ref="E106:H106"/>
-    <mergeCell ref="E95:H95"/>
-    <mergeCell ref="E96:H96"/>
-    <mergeCell ref="E97:H97"/>
-    <mergeCell ref="D98:H98"/>
-    <mergeCell ref="D99:H99"/>
-    <mergeCell ref="D100:H100"/>
-    <mergeCell ref="F90:H90"/>
-    <mergeCell ref="E91:H91"/>
-    <mergeCell ref="D92:H92"/>
-    <mergeCell ref="C93:H93"/>
-    <mergeCell ref="D94:H94"/>
-    <mergeCell ref="C103:H103"/>
-    <mergeCell ref="F85:H85"/>
-    <mergeCell ref="F84:H84"/>
-    <mergeCell ref="F86:H86"/>
-    <mergeCell ref="E87:H87"/>
-    <mergeCell ref="E88:H88"/>
-    <mergeCell ref="F89:H89"/>
-    <mergeCell ref="E78:H78"/>
-    <mergeCell ref="F79:H79"/>
-    <mergeCell ref="F80:H80"/>
-    <mergeCell ref="E81:H81"/>
-    <mergeCell ref="E82:H82"/>
-    <mergeCell ref="F83:H83"/>
-    <mergeCell ref="E72:H72"/>
-    <mergeCell ref="E73:H73"/>
-    <mergeCell ref="E74:H74"/>
-    <mergeCell ref="D75:H75"/>
-    <mergeCell ref="E76:H76"/>
-    <mergeCell ref="E77:H77"/>
-    <mergeCell ref="D62:H62"/>
-    <mergeCell ref="D63:H63"/>
-    <mergeCell ref="C68:H68"/>
-    <mergeCell ref="D69:H69"/>
-    <mergeCell ref="E70:H70"/>
-    <mergeCell ref="E71:H71"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="E61:H61"/>
-    <mergeCell ref="E50:H50"/>
-    <mergeCell ref="E51:H51"/>
-    <mergeCell ref="E52:H52"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="D44:H44"/>
-    <mergeCell ref="E45:H45"/>
-    <mergeCell ref="D46:H46"/>
-    <mergeCell ref="C47:H47"/>
-    <mergeCell ref="D48:H48"/>
-    <mergeCell ref="E49:H49"/>
-    <mergeCell ref="E38:H38"/>
-    <mergeCell ref="D39:H39"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="D41:H41"/>
-    <mergeCell ref="E42:H42"/>
-    <mergeCell ref="E43:H43"/>
-    <mergeCell ref="E31:H31"/>
-    <mergeCell ref="E32:H32"/>
-    <mergeCell ref="E34:H34"/>
-    <mergeCell ref="D35:H35"/>
-    <mergeCell ref="E36:H36"/>
-    <mergeCell ref="D37:H37"/>
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="E29:H29"/>
-    <mergeCell ref="E30:H30"/>
-    <mergeCell ref="D19:H19"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="D21:H21"/>
-    <mergeCell ref="D22:H22"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="D15:H15"/>
-    <mergeCell ref="D16:H16"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="D18:H18"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="B1:N1"/>
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="A109:G109"/>
+    <mergeCell ref="D107:G107"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="C65:G65"/>
+    <mergeCell ref="C66:G66"/>
+    <mergeCell ref="C67:G67"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="C102:G102"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="D105:G105"/>
+    <mergeCell ref="D106:G106"/>
+    <mergeCell ref="D95:G95"/>
+    <mergeCell ref="D96:G96"/>
+    <mergeCell ref="D97:G97"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="C99:G99"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="E90:G90"/>
+    <mergeCell ref="D91:G91"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="B93:G93"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="B103:G103"/>
+    <mergeCell ref="E85:G85"/>
+    <mergeCell ref="E84:G84"/>
+    <mergeCell ref="E86:G86"/>
+    <mergeCell ref="D87:G87"/>
+    <mergeCell ref="D88:G88"/>
+    <mergeCell ref="E89:G89"/>
+    <mergeCell ref="D78:G78"/>
+    <mergeCell ref="E79:G79"/>
+    <mergeCell ref="E80:G80"/>
+    <mergeCell ref="D81:G81"/>
+    <mergeCell ref="D82:G82"/>
+    <mergeCell ref="E83:G83"/>
+    <mergeCell ref="D72:G72"/>
+    <mergeCell ref="D73:G73"/>
+    <mergeCell ref="D74:G74"/>
+    <mergeCell ref="C75:G75"/>
+    <mergeCell ref="D76:G76"/>
+    <mergeCell ref="D77:G77"/>
+    <mergeCell ref="C62:G62"/>
+    <mergeCell ref="C63:G63"/>
+    <mergeCell ref="B68:G68"/>
+    <mergeCell ref="C69:G69"/>
+    <mergeCell ref="D70:G70"/>
+    <mergeCell ref="D71:G71"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="D50:G50"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="D52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="D42:G42"/>
+    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="D6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610B0901-B189-4E29-A796-4400F86449A9}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="24" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" s="22">
+        <v>160000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="22">
+        <v>22000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="22">
+        <v>158000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="24">
+        <v>15623000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="D6" s="24">
+        <v>282904000</v>
+      </c>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" s="24">
+        <v>2832000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" s="24">
+        <v>300000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D9" s="22">
+        <v>3450000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D10" s="22">
+        <v>31857000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D11" s="24">
+        <v>578983000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D12" s="24">
+        <v>55633000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="D13" s="24">
+        <v>2733000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D14" s="24">
+        <v>2297985000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D15" s="24">
+        <v>85121000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D16" s="24">
+        <v>79035000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" s="25">
+        <v>13711000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D18" s="25">
+        <v>84328000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="D25" s="25">
+        <v>3077392000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>